<commit_message>
Auto-committed on 2021/12/09 週四
Former-commit-id: 626636a9d70a1038d6fd5b551a13c348945c85e1
</commit_message>
<xml_diff>
--- a/Program/Other/URS會議審查紀錄/DbLayouts/L4-批次作業/BankRemit.xlsx
+++ b/Program/Other/URS會議審查紀錄/DbLayouts/L4-批次作業/BankRemit.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\SKL\DB\GenTables\L4-批次作業\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B37CAB-BEC1-4CE1-A8F7-E6AFFF346CD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077BD1D8-8D4E-4E3F-80E2-596CD9B84A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -489,14 +489,6 @@
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
-    <t>CdCode:DrawdownStatus
-0:正常
-1:產檔後修正
-2:產檔後訂正
-3.未放行(ActFg=1時顯示用)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>"LN + 傳票批號 + 匯款批號</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -507,6 +499,15 @@
 04:退款台新(存款憑條)
 05:退款他行(整批匯款)
 11:退款新光(存款憑條)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CdCode:DrawdownStatus
+0:正常
+1.未放行(ActFg=1時顯示用)
+2:產檔後訂正
+3:產檔後修正
+4.產檔後改單筆匯款</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1179,7 +1180,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:F7"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.44140625" defaultRowHeight="16.2"/>
@@ -1379,7 +1380,7 @@
       </c>
       <c r="F12" s="18"/>
       <c r="G12" s="34" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="97.2">
@@ -1400,10 +1401,10 @@
       </c>
       <c r="F13" s="18"/>
       <c r="G13" s="21" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="81">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="97.2">
       <c r="A14" s="18">
         <v>6</v>
       </c>
@@ -1421,7 +1422,7 @@
       </c>
       <c r="F14" s="18"/>
       <c r="G14" s="23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:7">

</xml_diff>

<commit_message>
Auto-committed on 2021/12/23 週四
Former-commit-id: cc6118ce87ad07971df116fe7583ccb33f2b14e0
</commit_message>
<xml_diff>
--- a/Program/Other/URS會議審查紀錄/DbLayouts/L4-批次作業/BankRemit.xlsx
+++ b/Program/Other/URS會議審查紀錄/DbLayouts/L4-批次作業/BankRemit.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\SKL\DB\GenTables\L4-批次作業\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077BD1D8-8D4E-4E3F-80E2-596CD9B84A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A135E04-B3F9-40E9-8C94-D74A9F97A6A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DBD" sheetId="1" r:id="rId1"/>
     <sheet name="DBS" sheetId="2" r:id="rId2"/>
     <sheet name="提出檔規格" sheetId="3" r:id="rId3"/>
+    <sheet name="回銷檔" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="229">
   <si>
     <t>SEQ</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -325,112 +326,7 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>Seq</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>EnglishColName</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>ChineseColName</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>Unit</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>Length</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>Start</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>Posision</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>Remark</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>DataSeq</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>序號</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>AcctNo</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>帳號</t>
-  </si>
-  <si>
     <t>X</t>
-  </si>
-  <si>
-    <t>Amount</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>金額</t>
-  </si>
-  <si>
-    <t>UnitCode</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>解付單位代號</t>
-  </si>
-  <si>
-    <t>RemitName</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>代償專戶</t>
-  </si>
-  <si>
-    <t>ColumnA</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>新光人壽保險股份有限公司─放款服務課</t>
-  </si>
-  <si>
-    <t>ColumnB</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>space</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>ColumnC</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>00174</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>RemitDate</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>匯款日期</t>
-  </si>
-  <si>
-    <t>BatchNo</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>批號</t>
   </si>
   <si>
     <t>findL4901B</t>
@@ -510,12 +406,608 @@
 4.產檔後改單筆匯款</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>付款狀況碼</t>
+  </si>
+  <si>
+    <t>付款狀況碼</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>PayCode</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>I:建檔
+O:確認
+C:建檔取消
+A:已開票
+D:支票到期
+B:退件
+S:請款單位擋匯
+T:網銀擋匯
+W:匯款途中
+F:匯款失敗
+H:支票兌領/匯款成功
+R:退匯/退回情況改變成作廢
+L:支票掛失
+V:支票作廢
+J:空白票遺失
+Z:逾一年未兌領
+Y:逾二年未兌領
+P:繳款成功
+X:付款沖回
+Q:AML相似名單確認中
+U:禁止交易(AML)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.頁面可以參考「費用付款作業」上傳作業 (格式同費用系統)</t>
+  </si>
+  <si>
+    <t>2.檔案格式：.csv,  編碼：UTF-8；欄位間以","進行區隔</t>
+  </si>
+  <si>
+    <t>Seq</t>
+  </si>
+  <si>
+    <t>Chinese Name</t>
+  </si>
+  <si>
+    <t>Data Type</t>
+  </si>
+  <si>
+    <t>Type
+Length</t>
+  </si>
+  <si>
+    <t>Nullable</t>
+  </si>
+  <si>
+    <t>說明</t>
+  </si>
+  <si>
+    <t>來源系統提供</t>
+  </si>
+  <si>
+    <r>
+      <t>請款序號</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t xml:space="preserve"> (PK)</t>
+    </r>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>核心押</t>
+  </si>
+  <si>
+    <t>空白</t>
+  </si>
+  <si>
+    <t>付款號碼</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>付款型態</t>
+  </si>
+  <si>
+    <t>核心押 E：手工請款</t>
+  </si>
+  <si>
+    <t>核心押 I：建檔</t>
+  </si>
+  <si>
+    <t>付款狀況異動日</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>核心押 上傳日期</t>
+  </si>
+  <si>
+    <t>付款方式</t>
+  </si>
+  <si>
+    <t>來源系統提供
+C:支票(銀行支票)
+R:匯款(銀行匯款/郵局匯款)</t>
+  </si>
+  <si>
+    <t>R:匯款(銀行匯款/郵局匯款)</t>
+  </si>
+  <si>
+    <t>付款處理(人工付款指示)</t>
+  </si>
+  <si>
+    <r>
+      <t>來源系統提供</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>A:非人工件</t>
+  </si>
+  <si>
+    <t>相關號碼</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">來源系統的key值
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>此欄不可重複，已取消匯款件除外</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">撥款:戶號-額度-撥款(15)
+退款:經辦(6)+交易序號(8)
+</t>
+  </si>
+  <si>
+    <t>受款人</t>
+  </si>
+  <si>
+    <t>受款人姓名</t>
+  </si>
+  <si>
+    <t>付款摘要</t>
+  </si>
+  <si>
+    <t>來源系統
+1~13碼為銷帳碼
+14~43碼為付款摘要</t>
+  </si>
+  <si>
+    <t>??待新壽確認</t>
+  </si>
+  <si>
+    <t>支票格式</t>
+  </si>
+  <si>
+    <t>來源系統提供（支票件）
+A: 畫線禁背
+B: 取消畫線
+C: 取消禁背</t>
+  </si>
+  <si>
+    <t>支票號碼</t>
+  </si>
+  <si>
+    <t>支票(匯款)日期</t>
+  </si>
+  <si>
+    <r>
+      <t>指定匯款日期，未指定則為上傳日期，</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>建議不指定。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="10"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>(民國年月日yyymmdd)</t>
+    </r>
+  </si>
+  <si>
+    <t>兌領日期</t>
+  </si>
+  <si>
+    <t>開票日期/匯款日期</t>
+  </si>
+  <si>
+    <t>受款總行</t>
+  </si>
+  <si>
+    <t>來源系統提供（匯款件）</t>
+  </si>
+  <si>
+    <t>受款銀行代號</t>
+  </si>
+  <si>
+    <t>受款分行</t>
+  </si>
+  <si>
+    <t>受款分行代號</t>
+  </si>
+  <si>
+    <t>受款人帳號</t>
+  </si>
+  <si>
+    <t>受款銀行帳號</t>
+  </si>
+  <si>
+    <t>付款金額</t>
+  </si>
+  <si>
+    <t>NUMBER</t>
+  </si>
+  <si>
+    <t>(12,2)</t>
+  </si>
+  <si>
+    <t>金額
+10位整數，2位小數；若為台幣無須提供小數位</t>
+  </si>
+  <si>
+    <t>程式代碼</t>
+  </si>
+  <si>
+    <t>核心押 hk504m</t>
+  </si>
+  <si>
+    <t>功能碼/變更項目別</t>
+  </si>
+  <si>
+    <t>作業者</t>
+  </si>
+  <si>
+    <t>核心押上傳者</t>
+  </si>
+  <si>
+    <t>作業日期</t>
+  </si>
+  <si>
+    <t>處理日期</t>
+  </si>
+  <si>
+    <t>核心押上傳日期</t>
+  </si>
+  <si>
+    <t>開票者/匯款者</t>
+  </si>
+  <si>
+    <t>請款單批號(付款憑單批號)</t>
+  </si>
+  <si>
+    <t>預設為0
+執行列印付款憑單時系統會取號</t>
+  </si>
+  <si>
+    <t>最近異動最遠票日</t>
+  </si>
+  <si>
+    <t>掛號型態</t>
+  </si>
+  <si>
+    <t>支票郵寄通知單型式</t>
+  </si>
+  <si>
+    <t>核心押 (支票件)
+center_ind = 1，則為A單位；否則為 3手工請款</t>
+  </si>
+  <si>
+    <t>郵寄標籤</t>
+  </si>
+  <si>
+    <t>郵寄通知人(單位)代號</t>
+  </si>
+  <si>
+    <t>請款單位代號</t>
+  </si>
+  <si>
+    <t>核心押上傳者的單位代號</t>
+  </si>
+  <si>
+    <t>扣匯款手續費</t>
+  </si>
+  <si>
+    <t>缺單據</t>
+  </si>
+  <si>
+    <t>缺單據原因</t>
+  </si>
+  <si>
+    <t>業務員代號</t>
+  </si>
+  <si>
+    <t>付款來源</t>
+  </si>
+  <si>
+    <t>核心應付作業負責人提供給來源系統
+來源系統提供</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t：放款系統(hk504m) </t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>傳輸匯款通知</t>
+  </si>
+  <si>
+    <t>傳輸匯款通知單位</t>
+  </si>
+  <si>
+    <t>匯款磁片編號</t>
+  </si>
+  <si>
+    <t>付款銀行</t>
+  </si>
+  <si>
+    <t>類別碼(簡碼)</t>
+  </si>
+  <si>
+    <t>支票郵寄日</t>
+  </si>
+  <si>
+    <t>入帳號碼</t>
+  </si>
+  <si>
+    <t>到期作業指示</t>
+  </si>
+  <si>
+    <t>郵遞區號</t>
+  </si>
+  <si>
+    <t>寄達地址</t>
+  </si>
+  <si>
+    <t>付款開票格式</t>
+  </si>
+  <si>
+    <t>受款人ID</t>
+  </si>
+  <si>
+    <t>受款人的身分證字號</t>
+  </si>
+  <si>
+    <t>前期建檔號碼</t>
+  </si>
+  <si>
+    <t>付款單位代送</t>
+  </si>
+  <si>
+    <r>
+      <t>核心押
+支票件 1:單位轉送
+匯款件 0:非單位轉送</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>取消建檔原因碼</t>
+  </si>
+  <si>
+    <t>群組請款序號</t>
+  </si>
+  <si>
+    <t>合併付款群組號碼</t>
+  </si>
+  <si>
+    <t>合併欄位</t>
+  </si>
+  <si>
+    <t>若需合併給付此欄位需放一樣的值</t>
+  </si>
+  <si>
+    <t>權責單位(請款單位)覆核日</t>
+  </si>
+  <si>
+    <t>權責單位(請款單位)覆核者</t>
+  </si>
+  <si>
+    <t>付款單位(出納)覆核日</t>
+  </si>
+  <si>
+    <t>付款單位(出納)覆核者</t>
+  </si>
+  <si>
+    <t>服務中心-匯款彙總批號</t>
+  </si>
+  <si>
+    <t>付款單位-覆核批號</t>
+  </si>
+  <si>
+    <t>帳號錯誤通知單位/人</t>
+  </si>
+  <si>
+    <t>來源系統提供(帳冊幣別)</t>
+  </si>
+  <si>
+    <t>匯款幣別(一律台幣件)</t>
+  </si>
+  <si>
+    <t>NTD</t>
+  </si>
+  <si>
+    <t>櫃檯支票簽收類別</t>
+  </si>
+  <si>
+    <t>核心押0:不需要簽收</t>
+  </si>
+  <si>
+    <t>櫃檯支票簽收者ID</t>
+  </si>
+  <si>
+    <t>櫃檯支票簽收者姓名</t>
+  </si>
+  <si>
+    <t>批次櫃台指示碼(件類別)</t>
+  </si>
+  <si>
+    <t>核心押1:批次</t>
+  </si>
+  <si>
+    <t>支票寄達單位</t>
+  </si>
+  <si>
+    <t>批號付款序號</t>
+  </si>
+  <si>
+    <t>檔案格式：.csv</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>欄位中文名稱</t>
+  </si>
+  <si>
+    <t>資料類型</t>
+  </si>
+  <si>
+    <t>格式</t>
+  </si>
+  <si>
+    <t>請款序號</t>
+  </si>
+  <si>
+    <t>字元</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>I:建檔
+O:確認
+C:建檔取消</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t xml:space="preserve">
+A:已開票
+D:支票到期
+B:退件
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>S:請款單位擋匯
+T:網銀擋匯
+W:匯款途中</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t xml:space="preserve">
+F:匯款失敗
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>H:支票兌領/匯款成功
+R:退匯/退回情況改變成作廢</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t xml:space="preserve">
+L:支票掛失
+V:支票作廢
+J:空白票遺失
+Z:逾一年未兌領
+Y:逾二年未兌領
+P:繳款成功
+X:付款沖回
+Q:AML相似名單確認中
+U:禁止交易(AML)</t>
+    </r>
+  </si>
+  <si>
+    <t>yyymmdd</t>
+  </si>
+  <si>
+    <t>民國年</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <numFmts count="1">
+    <numFmt numFmtId="180" formatCode="#,##0_ "/>
+  </numFmts>
+  <fonts count="28">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -604,21 +1096,115 @@
       <charset val="136"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
-      <color theme="1"/>
+      <color indexed="8"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="微軟正黑體"/>
       <family val="2"/>
       <charset val="136"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="新細明體"/>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="微軟正黑體"/>
       <family val="2"/>
       <charset val="136"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="微軟正黑體"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="9"/>
+      <name val="微軟正黑體"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="微軟正黑體"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="微軟正黑體"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="10"/>
+      <name val="微軟正黑體"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="微軟正黑體"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="9"/>
+      <name val="微軟正黑體"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0070C0"/>
+      <name val="微軟正黑體"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="微軟正黑體"/>
+      <family val="2"/>
+      <charset val="136"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -631,8 +1217,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="12"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -696,10 +1294,85 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -708,7 +1381,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -718,8 +1391,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -804,21 +1485,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -837,11 +1503,167 @@
     <xf numFmtId="49" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="6" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="8" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="8" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="5" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="17" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="5" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="4" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="5" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="17" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="7">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
     <cellStyle name="一般 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="一般 2 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="一般 2 3" xfId="4" xr:uid="{6DE46EBB-7A13-49D9-A09F-09A939E7A3F1}"/>
+    <cellStyle name="一般 3" xfId="5" xr:uid="{3633756A-793B-4CC6-8F8D-D5F8154DE244}"/>
+    <cellStyle name="一般 4" xfId="3" xr:uid="{12658DE8-C825-471B-9699-BE248273D873}"/>
+    <cellStyle name="一般_Sheet1" xfId="6" xr:uid="{B60F5320-A7B8-4393-A37F-6A284E96C5D5}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1177,10 +1999,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.44140625" defaultRowHeight="16.2"/>
@@ -1195,10 +2017,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="36"/>
+      <c r="B1" s="31"/>
       <c r="C1" s="3" t="s">
         <v>45</v>
       </c>
@@ -1210,8 +2032,8 @@
       <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="35"/>
-      <c r="B2" s="36"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="31"/>
       <c r="C2" s="7" t="s">
         <v>74</v>
       </c>
@@ -1223,12 +2045,12 @@
       <c r="G2" s="10"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="38"/>
+      <c r="B3" s="33"/>
       <c r="C3" s="11" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>17</v>
@@ -1238,10 +2060,10 @@
       <c r="G3" s="10"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="37"/>
+      <c r="B4" s="32"/>
       <c r="C4" s="11"/>
       <c r="D4" s="12"/>
       <c r="E4" s="9"/>
@@ -1249,10 +2071,10 @@
       <c r="G4" s="10"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="38"/>
+      <c r="B5" s="33"/>
       <c r="C5" s="11" t="s">
         <v>56</v>
       </c>
@@ -1262,10 +2084,10 @@
       <c r="G5" s="10"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="31"/>
       <c r="C6" s="3"/>
       <c r="D6" s="12"/>
       <c r="E6" s="9"/>
@@ -1273,10 +2095,10 @@
       <c r="G6" s="10"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="37"/>
+      <c r="B7" s="32"/>
       <c r="C7" s="3"/>
       <c r="D7" s="12"/>
       <c r="E7" s="9"/>
@@ -1367,7 +2189,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>115</v>
+        <v>87</v>
       </c>
       <c r="C12" s="19" t="s">
         <v>20</v>
@@ -1379,8 +2201,8 @@
         <v>6</v>
       </c>
       <c r="F12" s="18"/>
-      <c r="G12" s="34" t="s">
-        <v>121</v>
+      <c r="G12" s="29" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="97.2">
@@ -1401,7 +2223,7 @@
       </c>
       <c r="F13" s="18"/>
       <c r="G13" s="21" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="97.2">
@@ -1412,7 +2234,7 @@
         <v>50</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>109</v>
+        <v>81</v>
       </c>
       <c r="D14" s="18" t="s">
         <v>40</v>
@@ -1422,7 +2244,7 @@
       </c>
       <c r="F14" s="18"/>
       <c r="G14" s="23" t="s">
-        <v>123</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1592,7 +2414,7 @@
         <v>16</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>113</v>
+        <v>85</v>
       </c>
       <c r="C24" s="19" t="s">
         <v>28</v>
@@ -1624,8 +2446,8 @@
         <v>1</v>
       </c>
       <c r="F25" s="22"/>
-      <c r="G25" s="33" t="s">
-        <v>111</v>
+      <c r="G25" s="28" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="32.4">
@@ -1633,20 +2455,20 @@
         <v>18</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>118</v>
+        <v>90</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
       <c r="E26" s="18">
         <v>1</v>
       </c>
       <c r="F26" s="18"/>
-      <c r="G26" s="33" t="s">
-        <v>112</v>
+      <c r="G26" s="28" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1654,10 +2476,10 @@
         <v>19</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>114</v>
+        <v>86</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>119</v>
+        <v>91</v>
       </c>
       <c r="D27" s="18" t="s">
         <v>42</v>
@@ -1666,61 +2488,65 @@
         <v>500</v>
       </c>
       <c r="F27" s="18"/>
-      <c r="G27" s="34" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
+      <c r="G27" s="29" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="340.2">
       <c r="A28" s="18">
         <v>20</v>
       </c>
-      <c r="B28" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="C28" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="D28" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="E28" s="20"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="33"/>
+      <c r="B28" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E28" s="18">
+        <v>1</v>
+      </c>
+      <c r="F28" s="18"/>
+      <c r="G28" s="23" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="18">
         <v>21</v>
       </c>
       <c r="B29" s="25" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C29" s="26" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D29" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="E29" s="20">
-        <v>6</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="E29" s="20"/>
       <c r="F29" s="22"/>
       <c r="G29" s="27"/>
+      <c r="H29" s="28"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="18">
         <v>22</v>
       </c>
       <c r="B30" s="25" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C30" s="26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D30" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="E30" s="20"/>
+        <v>68</v>
+      </c>
+      <c r="E30" s="20">
+        <v>6</v>
+      </c>
       <c r="F30" s="22"/>
       <c r="G30" s="27"/>
     </row>
@@ -1729,19 +2555,36 @@
         <v>23</v>
       </c>
       <c r="B31" s="25" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C31" s="26" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D31" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="E31" s="20">
-        <v>6</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="E31" s="20"/>
       <c r="F31" s="22"/>
       <c r="G31" s="27"/>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="18">
+        <v>24</v>
+      </c>
+      <c r="B32" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="D32" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="E32" s="20">
+        <v>6</v>
+      </c>
+      <c r="F32" s="22"/>
+      <c r="G32" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1805,7 +2648,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>108</v>
+        <v>80</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>76</v>
@@ -1834,309 +2677,1969 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2"/>
   <cols>
-    <col min="1" max="1" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.109375" customWidth="1"/>
+    <col min="2" max="2" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.8" thickBot="1">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="53" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+    </row>
+    <row r="2" spans="1:8" ht="16.8" thickBot="1">
+      <c r="A2" s="53" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+    </row>
+    <row r="3" spans="1:8" ht="41.4">
+      <c r="A3" s="47" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="48" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="E3" s="50" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3" s="51" t="s">
+        <v>107</v>
+      </c>
+      <c r="G3" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="H3" s="52"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="54">
+        <v>1</v>
+      </c>
+      <c r="B4" s="55" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="56">
+        <v>12</v>
+      </c>
+      <c r="E4" s="57" t="s">
+        <v>110</v>
+      </c>
+      <c r="F4" s="58" t="s">
+        <v>111</v>
+      </c>
+      <c r="G4" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H4" s="38"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="54">
+        <v>2</v>
+      </c>
+      <c r="B5" s="55" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="56">
+        <v>12</v>
+      </c>
+      <c r="E5" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F5" s="58" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="G5" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H5" s="39"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="54">
+        <v>3</v>
+      </c>
+      <c r="B6" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="56">
+        <v>1</v>
+      </c>
+      <c r="E6" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F6" s="58" t="s">
+        <v>116</v>
+      </c>
+      <c r="G6" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H6" s="39"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="54">
+        <v>4</v>
+      </c>
+      <c r="B7" s="55" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="56">
+        <v>1</v>
+      </c>
+      <c r="E7" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F7" s="58" t="s">
+        <v>117</v>
+      </c>
+      <c r="G7" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H7" s="39"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="54">
+        <v>5</v>
+      </c>
+      <c r="B8" s="55" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" s="55" t="s">
+        <v>119</v>
+      </c>
+      <c r="D8" s="56">
+        <v>7</v>
+      </c>
+      <c r="E8" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F8" s="58" t="s">
+        <v>120</v>
+      </c>
+      <c r="G8" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H8" s="39"/>
+    </row>
+    <row r="9" spans="1:8" ht="165.6">
+      <c r="A9" s="59">
+        <v>6</v>
+      </c>
+      <c r="B9" s="60" t="s">
+        <v>121</v>
+      </c>
+      <c r="C9" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="61">
+        <v>1</v>
+      </c>
+      <c r="E9" s="62" t="s">
+        <v>114</v>
+      </c>
+      <c r="F9" s="63" t="s">
+        <v>122</v>
+      </c>
+      <c r="G9" s="40" t="s">
+        <v>123</v>
+      </c>
+      <c r="H9" s="39"/>
+    </row>
+    <row r="10" spans="1:8" ht="41.4">
+      <c r="A10" s="59">
+        <v>7</v>
+      </c>
+      <c r="B10" s="60" t="s">
+        <v>124</v>
+      </c>
+      <c r="C10" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="61">
+        <v>1</v>
+      </c>
+      <c r="E10" s="62" t="s">
+        <v>114</v>
+      </c>
+      <c r="F10" s="63" t="s">
+        <v>125</v>
+      </c>
+      <c r="G10" s="40" t="s">
+        <v>126</v>
+      </c>
+      <c r="H10" s="39"/>
+    </row>
+    <row r="11" spans="1:8" ht="96.6">
+      <c r="A11" s="59">
+        <v>8</v>
+      </c>
+      <c r="B11" s="60" t="s">
+        <v>127</v>
+      </c>
+      <c r="C11" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="61">
+        <v>15</v>
+      </c>
+      <c r="E11" s="62" t="s">
+        <v>114</v>
+      </c>
+      <c r="F11" s="64" t="s">
+        <v>108</v>
+      </c>
+      <c r="G11" s="40" t="s">
+        <v>128</v>
+      </c>
+      <c r="H11" s="41" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="59">
+        <v>9</v>
+      </c>
+      <c r="B12" s="60" t="s">
+        <v>130</v>
+      </c>
+      <c r="C12" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="61">
+        <v>40</v>
+      </c>
+      <c r="E12" s="62" t="s">
+        <v>114</v>
+      </c>
+      <c r="F12" s="64" t="s">
+        <v>108</v>
+      </c>
+      <c r="G12" s="40" t="s">
+        <v>131</v>
+      </c>
+      <c r="H12" s="39"/>
+    </row>
+    <row r="13" spans="1:8" ht="69">
+      <c r="A13" s="59">
+        <v>10</v>
+      </c>
+      <c r="B13" s="60" t="s">
+        <v>132</v>
+      </c>
+      <c r="C13" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="61">
+        <v>45</v>
+      </c>
+      <c r="E13" s="62" t="s">
+        <v>114</v>
+      </c>
+      <c r="F13" s="64" t="s">
+        <v>108</v>
+      </c>
+      <c r="G13" s="42" t="s">
+        <v>133</v>
+      </c>
+      <c r="H13" s="39" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="220.8">
+      <c r="A14" s="59">
+        <v>11</v>
+      </c>
+      <c r="B14" s="60" t="s">
+        <v>135</v>
+      </c>
+      <c r="C14" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="61">
+        <v>1</v>
+      </c>
+      <c r="E14" s="65" t="s">
+        <v>114</v>
+      </c>
+      <c r="F14" s="63" t="s">
+        <v>136</v>
+      </c>
+      <c r="G14" s="40" t="s">
+        <v>112</v>
+      </c>
+      <c r="H14" s="41"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="54">
+        <v>12</v>
+      </c>
+      <c r="B15" s="55" t="s">
+        <v>137</v>
+      </c>
+      <c r="C15" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="56">
+        <v>9</v>
+      </c>
+      <c r="E15" s="66" t="s">
+        <v>114</v>
+      </c>
+      <c r="F15" s="58" t="s">
+        <v>79</v>
+      </c>
+      <c r="G15" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H15" s="39"/>
+    </row>
+    <row r="16" spans="1:8" ht="124.2">
+      <c r="A16" s="59">
+        <v>13</v>
+      </c>
+      <c r="B16" s="60" t="s">
+        <v>138</v>
+      </c>
+      <c r="C16" s="60" t="s">
+        <v>119</v>
+      </c>
+      <c r="D16" s="61">
+        <v>7</v>
+      </c>
+      <c r="E16" s="65" t="s">
+        <v>114</v>
+      </c>
+      <c r="F16" s="64" t="s">
+        <v>108</v>
+      </c>
+      <c r="G16" s="40" t="s">
+        <v>139</v>
+      </c>
+      <c r="H16" s="39" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="54">
+        <v>14</v>
+      </c>
+      <c r="B17" s="55" t="s">
+        <v>140</v>
+      </c>
+      <c r="C17" s="55" t="s">
+        <v>119</v>
+      </c>
+      <c r="D17" s="56">
+        <v>7</v>
+      </c>
+      <c r="E17" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F17" s="58" t="s">
+        <v>79</v>
+      </c>
+      <c r="G17" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H17" s="39"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="54">
+        <v>15</v>
+      </c>
+      <c r="B18" s="55" t="s">
+        <v>141</v>
+      </c>
+      <c r="C18" s="55" t="s">
+        <v>119</v>
+      </c>
+      <c r="D18" s="56">
+        <v>7</v>
+      </c>
+      <c r="E18" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F18" s="58" t="s">
+        <v>79</v>
+      </c>
+      <c r="G18" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H18" s="39"/>
+    </row>
+    <row r="19" spans="1:8" ht="27.6">
+      <c r="A19" s="59">
+        <v>16</v>
+      </c>
+      <c r="B19" s="60" t="s">
+        <v>142</v>
+      </c>
+      <c r="C19" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="61">
+        <v>3</v>
+      </c>
+      <c r="E19" s="62" t="s">
+        <v>114</v>
+      </c>
+      <c r="F19" s="64" t="s">
+        <v>143</v>
+      </c>
+      <c r="G19" s="40" t="s">
+        <v>144</v>
+      </c>
+      <c r="H19" s="39"/>
+    </row>
+    <row r="20" spans="1:8" ht="27.6">
+      <c r="A20" s="59">
+        <v>17</v>
+      </c>
+      <c r="B20" s="60" t="s">
+        <v>145</v>
+      </c>
+      <c r="C20" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="61">
+        <v>4</v>
+      </c>
+      <c r="E20" s="62" t="s">
+        <v>114</v>
+      </c>
+      <c r="F20" s="64" t="s">
+        <v>143</v>
+      </c>
+      <c r="G20" s="40" t="s">
+        <v>146</v>
+      </c>
+      <c r="H20" s="39"/>
+    </row>
+    <row r="21" spans="1:8" ht="27.6">
+      <c r="A21" s="59">
+        <v>18</v>
+      </c>
+      <c r="B21" s="60" t="s">
+        <v>147</v>
+      </c>
+      <c r="C21" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="61">
+        <v>16</v>
+      </c>
+      <c r="E21" s="62" t="s">
+        <v>114</v>
+      </c>
+      <c r="F21" s="64" t="s">
+        <v>143</v>
+      </c>
+      <c r="G21" s="40" t="s">
+        <v>148</v>
+      </c>
+      <c r="H21" s="39"/>
+    </row>
+    <row r="22" spans="1:8" ht="82.8">
+      <c r="A22" s="59">
+        <v>19</v>
+      </c>
+      <c r="B22" s="60" t="s">
+        <v>149</v>
+      </c>
+      <c r="C22" s="60" t="s">
+        <v>150</v>
+      </c>
+      <c r="D22" s="67" t="s">
+        <v>151</v>
+      </c>
+      <c r="E22" s="62" t="s">
+        <v>114</v>
+      </c>
+      <c r="F22" s="64" t="s">
+        <v>108</v>
+      </c>
+      <c r="G22" s="40" t="s">
+        <v>152</v>
+      </c>
+      <c r="H22" s="39"/>
+    </row>
+    <row r="23" spans="1:8" ht="55.2">
+      <c r="A23" s="54">
+        <v>20</v>
+      </c>
+      <c r="B23" s="55" t="s">
+        <v>153</v>
+      </c>
+      <c r="C23" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="56">
+        <v>8</v>
+      </c>
+      <c r="E23" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F23" s="68" t="s">
+        <v>154</v>
+      </c>
+      <c r="G23" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H23" s="39"/>
+    </row>
+    <row r="24" spans="1:8" ht="27.6">
+      <c r="A24" s="54">
+        <v>21</v>
+      </c>
+      <c r="B24" s="55" t="s">
+        <v>155</v>
+      </c>
+      <c r="C24" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="56">
+        <v>2</v>
+      </c>
+      <c r="E24" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F24" s="68" t="s">
+        <v>111</v>
+      </c>
+      <c r="G24" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H24" s="39"/>
+    </row>
+    <row r="25" spans="1:8" ht="41.4">
+      <c r="A25" s="54">
+        <v>22</v>
+      </c>
+      <c r="B25" s="55" t="s">
+        <v>156</v>
+      </c>
+      <c r="C25" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="56">
+        <v>8</v>
+      </c>
+      <c r="E25" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F25" s="68" t="s">
+        <v>157</v>
+      </c>
+      <c r="G25" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H25" s="39"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="54">
+        <v>23</v>
+      </c>
+      <c r="B26" s="55" t="s">
+        <v>158</v>
+      </c>
+      <c r="C26" s="55" t="s">
+        <v>119</v>
+      </c>
+      <c r="D26" s="56">
+        <v>7</v>
+      </c>
+      <c r="E26" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F26" s="68" t="s">
+        <v>79</v>
+      </c>
+      <c r="G26" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H26" s="34"/>
+    </row>
+    <row r="27" spans="1:8" ht="55.2">
+      <c r="A27" s="54">
+        <v>24</v>
+      </c>
+      <c r="B27" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="C27" s="55" t="s">
+        <v>119</v>
+      </c>
+      <c r="D27" s="56">
+        <v>7</v>
+      </c>
+      <c r="E27" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F27" s="68" t="s">
+        <v>160</v>
+      </c>
+      <c r="G27" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H27" s="34"/>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="54">
+        <v>25</v>
+      </c>
+      <c r="B28" s="55" t="s">
+        <v>161</v>
+      </c>
+      <c r="C28" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" s="56">
+        <v>8</v>
+      </c>
+      <c r="E28" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F28" s="68" t="s">
+        <v>79</v>
+      </c>
+      <c r="G28" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H28" s="39"/>
+    </row>
+    <row r="29" spans="1:8" ht="124.2">
+      <c r="A29" s="54">
+        <v>26</v>
+      </c>
+      <c r="B29" s="55" t="s">
+        <v>162</v>
+      </c>
+      <c r="C29" s="55" t="s">
+        <v>150</v>
+      </c>
+      <c r="D29" s="56">
+        <v>10</v>
+      </c>
+      <c r="E29" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F29" s="68" t="s">
+        <v>163</v>
+      </c>
+      <c r="G29" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H29" s="39"/>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="54">
+        <v>27</v>
+      </c>
+      <c r="B30" s="55" t="s">
+        <v>164</v>
+      </c>
+      <c r="C30" s="55" t="s">
+        <v>119</v>
+      </c>
+      <c r="D30" s="56">
+        <v>7</v>
+      </c>
+      <c r="E30" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F30" s="68" t="s">
+        <v>79</v>
+      </c>
+      <c r="G30" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H30" s="39"/>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="54">
+        <v>28</v>
+      </c>
+      <c r="B31" s="55" t="s">
+        <v>165</v>
+      </c>
+      <c r="C31" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="D31" s="56">
+        <v>1</v>
+      </c>
+      <c r="E31" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F31" s="68" t="s">
+        <v>79</v>
+      </c>
+      <c r="G31" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H31" s="39"/>
+    </row>
+    <row r="32" spans="1:8" ht="165.6">
+      <c r="A32" s="54">
+        <v>29</v>
+      </c>
+      <c r="B32" s="55" t="s">
+        <v>166</v>
+      </c>
+      <c r="C32" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32" s="56">
+        <v>1</v>
+      </c>
+      <c r="E32" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F32" s="68" t="s">
+        <v>167</v>
+      </c>
+      <c r="G32" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H32" s="39"/>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="54">
+        <v>30</v>
+      </c>
+      <c r="B33" s="55" t="s">
+        <v>168</v>
+      </c>
+      <c r="C33" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="D33" s="56">
+        <v>1</v>
+      </c>
+      <c r="E33" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F33" s="68" t="s">
+        <v>79</v>
+      </c>
+      <c r="G33" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H33" s="39"/>
+    </row>
+    <row r="34" spans="1:8" ht="220.8">
+      <c r="A34" s="59">
+        <v>31</v>
+      </c>
+      <c r="B34" s="60" t="s">
+        <v>169</v>
+      </c>
+      <c r="C34" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" s="61">
+        <v>12</v>
+      </c>
+      <c r="E34" s="62" t="s">
+        <v>114</v>
+      </c>
+      <c r="F34" s="63" t="s">
+        <v>136</v>
+      </c>
+      <c r="G34" s="40" t="s">
+        <v>112</v>
+      </c>
+      <c r="H34" s="39"/>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="54">
+        <v>32</v>
+      </c>
+      <c r="B35" s="55" t="s">
+        <v>170</v>
+      </c>
+      <c r="C35" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="D35" s="56">
+        <v>6</v>
+      </c>
+      <c r="E35" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F35" s="58" t="s">
+        <v>171</v>
+      </c>
+      <c r="G35" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H35" s="39"/>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="54">
+        <v>33</v>
+      </c>
+      <c r="B36" s="55" t="s">
+        <v>172</v>
+      </c>
+      <c r="C36" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="D36" s="56">
+        <v>1</v>
+      </c>
+      <c r="E36" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F36" s="58" t="s">
+        <v>79</v>
+      </c>
+      <c r="G36" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H36" s="39"/>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="54">
+        <v>34</v>
+      </c>
+      <c r="B37" s="55" t="s">
+        <v>173</v>
+      </c>
+      <c r="C37" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="D37" s="56">
+        <v>1</v>
+      </c>
+      <c r="E37" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F37" s="68" t="s">
+        <v>79</v>
+      </c>
+      <c r="G37" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H37" s="39"/>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="54">
+        <v>35</v>
+      </c>
+      <c r="B38" s="55" t="s">
+        <v>174</v>
+      </c>
+      <c r="C38" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="D38" s="56">
+        <v>1</v>
+      </c>
+      <c r="E38" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F38" s="68" t="s">
+        <v>79</v>
+      </c>
+      <c r="G38" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H38" s="39"/>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="54">
+        <v>36</v>
+      </c>
+      <c r="B39" s="55" t="s">
+        <v>175</v>
+      </c>
+      <c r="C39" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="D39" s="56">
+        <v>12</v>
+      </c>
+      <c r="E39" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F39" s="58" t="s">
+        <v>79</v>
+      </c>
+      <c r="G39" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H39" s="39"/>
+    </row>
+    <row r="40" spans="1:8" ht="151.80000000000001">
+      <c r="A40" s="59">
+        <v>37</v>
+      </c>
+      <c r="B40" s="60" t="s">
+        <v>176</v>
+      </c>
+      <c r="C40" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="D40" s="61">
+        <v>1</v>
+      </c>
+      <c r="E40" s="62" t="s">
+        <v>114</v>
+      </c>
+      <c r="F40" s="63" t="s">
+        <v>177</v>
+      </c>
+      <c r="G40" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="H40" s="38" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="54">
+        <v>38</v>
+      </c>
+      <c r="B41" s="55" t="s">
+        <v>180</v>
+      </c>
+      <c r="C41" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="D41" s="56">
+        <v>1</v>
+      </c>
+      <c r="E41" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F41" s="68" t="s">
+        <v>79</v>
+      </c>
+      <c r="G41" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H41" s="39"/>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="54">
+        <v>39</v>
+      </c>
+      <c r="B42" s="55" t="s">
+        <v>181</v>
+      </c>
+      <c r="C42" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="D42" s="56">
+        <v>6</v>
+      </c>
+      <c r="E42" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F42" s="68" t="s">
+        <v>79</v>
+      </c>
+      <c r="G42" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H42" s="39"/>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="54">
+        <v>40</v>
+      </c>
+      <c r="B43" s="55" t="s">
+        <v>182</v>
+      </c>
+      <c r="C43" s="55" t="s">
+        <v>150</v>
+      </c>
+      <c r="D43" s="56">
+        <v>10</v>
+      </c>
+      <c r="E43" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F43" s="58" t="s">
+        <v>79</v>
+      </c>
+      <c r="G43" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H43" s="39"/>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" s="54">
+        <v>41</v>
+      </c>
+      <c r="B44" s="55" t="s">
+        <v>183</v>
+      </c>
+      <c r="C44" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="D44" s="56">
+        <v>7</v>
+      </c>
+      <c r="E44" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F44" s="58" t="s">
+        <v>79</v>
+      </c>
+      <c r="G44" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H44" s="39"/>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" s="54">
+        <v>42</v>
+      </c>
+      <c r="B45" s="55" t="s">
+        <v>184</v>
+      </c>
+      <c r="C45" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="D45" s="56">
+        <v>10</v>
+      </c>
+      <c r="E45" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F45" s="58" t="s">
+        <v>79</v>
+      </c>
+      <c r="G45" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H45" s="39"/>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" s="54">
+        <v>43</v>
+      </c>
+      <c r="B46" s="55" t="s">
+        <v>185</v>
+      </c>
+      <c r="C46" s="55" t="s">
+        <v>119</v>
+      </c>
+      <c r="D46" s="56">
+        <v>7</v>
+      </c>
+      <c r="E46" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F46" s="58" t="s">
+        <v>79</v>
+      </c>
+      <c r="G46" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H46" s="39"/>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" s="54">
+        <v>44</v>
+      </c>
+      <c r="B47" s="55" t="s">
+        <v>186</v>
+      </c>
+      <c r="C47" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="D47" s="56">
+        <v>12</v>
+      </c>
+      <c r="E47" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F47" s="58" t="s">
+        <v>79</v>
+      </c>
+      <c r="G47" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H47" s="39"/>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="54">
+        <v>45</v>
+      </c>
+      <c r="B48" s="55" t="s">
+        <v>187</v>
+      </c>
+      <c r="C48" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="D48" s="56">
+        <v>1</v>
+      </c>
+      <c r="E48" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F48" s="68" t="s">
+        <v>79</v>
+      </c>
+      <c r="G48" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H48" s="39"/>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="54">
+        <v>46</v>
+      </c>
+      <c r="B49" s="55" t="s">
+        <v>188</v>
+      </c>
+      <c r="C49" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="D49" s="56">
+        <v>5</v>
+      </c>
+      <c r="E49" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F49" s="58" t="s">
+        <v>79</v>
+      </c>
+      <c r="G49" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H49" s="39"/>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" s="54">
+        <v>47</v>
+      </c>
+      <c r="B50" s="55" t="s">
+        <v>189</v>
+      </c>
+      <c r="C50" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="D50" s="56">
         <v>80</v>
       </c>
-      <c r="C1" s="28" t="s">
-        <v>81</v>
-      </c>
-      <c r="D1" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="E1" s="28" t="s">
-        <v>83</v>
-      </c>
-      <c r="F1" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="G1" s="28" t="s">
-        <v>85</v>
-      </c>
-      <c r="H1" s="29" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="31">
+      <c r="E50" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F50" s="58" t="s">
+        <v>79</v>
+      </c>
+      <c r="G50" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H50" s="39"/>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" s="54">
+        <v>48</v>
+      </c>
+      <c r="B51" s="55" t="s">
+        <v>190</v>
+      </c>
+      <c r="C51" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="D51" s="56">
         <v>1</v>
       </c>
-      <c r="B2" s="31" t="s">
-        <v>87</v>
-      </c>
-      <c r="C2" s="31" t="s">
-        <v>88</v>
-      </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31">
+      <c r="E51" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F51" s="68" t="s">
+        <v>79</v>
+      </c>
+      <c r="G51" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H51" s="39"/>
+    </row>
+    <row r="52" spans="1:8" ht="27.6">
+      <c r="A52" s="59">
+        <v>49</v>
+      </c>
+      <c r="B52" s="60" t="s">
+        <v>191</v>
+      </c>
+      <c r="C52" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="D52" s="61">
+        <v>10</v>
+      </c>
+      <c r="E52" s="62" t="s">
+        <v>114</v>
+      </c>
+      <c r="F52" s="64" t="s">
+        <v>108</v>
+      </c>
+      <c r="G52" s="40" t="s">
+        <v>192</v>
+      </c>
+      <c r="H52" s="39"/>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" s="54">
+        <v>50</v>
+      </c>
+      <c r="B53" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="C53" s="69" t="s">
+        <v>41</v>
+      </c>
+      <c r="D53" s="56">
+        <v>12</v>
+      </c>
+      <c r="E53" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F53" s="58" t="s">
+        <v>79</v>
+      </c>
+      <c r="G53" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H53" s="39"/>
+    </row>
+    <row r="54" spans="1:8" ht="151.80000000000001">
+      <c r="A54" s="54">
+        <v>51</v>
+      </c>
+      <c r="B54" s="55" t="s">
+        <v>194</v>
+      </c>
+      <c r="C54" s="69" t="s">
+        <v>41</v>
+      </c>
+      <c r="D54" s="56">
+        <v>1</v>
+      </c>
+      <c r="E54" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F54" s="68" t="s">
+        <v>195</v>
+      </c>
+      <c r="G54" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H54" s="39"/>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" s="54">
+        <v>52</v>
+      </c>
+      <c r="B55" s="55" t="s">
+        <v>196</v>
+      </c>
+      <c r="C55" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="D55" s="56">
+        <v>2</v>
+      </c>
+      <c r="E55" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F55" s="68" t="s">
+        <v>79</v>
+      </c>
+      <c r="G55" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H55" s="39"/>
+    </row>
+    <row r="56" spans="1:8" ht="27.6">
+      <c r="A56" s="54">
+        <v>53</v>
+      </c>
+      <c r="B56" s="54" t="s">
+        <v>197</v>
+      </c>
+      <c r="C56" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="D56" s="70">
+        <v>12</v>
+      </c>
+      <c r="E56" s="57" t="s">
+        <v>110</v>
+      </c>
+      <c r="F56" s="68" t="s">
+        <v>111</v>
+      </c>
+      <c r="G56" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H56" s="39"/>
+    </row>
+    <row r="57" spans="1:8" ht="41.4">
+      <c r="A57" s="59">
+        <v>54</v>
+      </c>
+      <c r="B57" s="60" t="s">
+        <v>198</v>
+      </c>
+      <c r="C57" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="D57" s="61">
+        <v>12</v>
+      </c>
+      <c r="E57" s="62" t="s">
+        <v>114</v>
+      </c>
+      <c r="F57" s="64" t="s">
+        <v>199</v>
+      </c>
+      <c r="G57" s="40" t="s">
+        <v>200</v>
+      </c>
+      <c r="H57" s="39" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" s="54">
+        <v>55</v>
+      </c>
+      <c r="B58" s="55" t="s">
+        <v>201</v>
+      </c>
+      <c r="C58" s="55" t="s">
+        <v>119</v>
+      </c>
+      <c r="D58" s="56">
+        <v>7</v>
+      </c>
+      <c r="E58" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F58" s="68" t="s">
+        <v>79</v>
+      </c>
+      <c r="G58" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H58" s="39"/>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59" s="54">
+        <v>56</v>
+      </c>
+      <c r="B59" s="55" t="s">
+        <v>202</v>
+      </c>
+      <c r="C59" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="D59" s="56">
+        <v>8</v>
+      </c>
+      <c r="E59" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F59" s="68" t="s">
+        <v>79</v>
+      </c>
+      <c r="G59" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H59" s="39"/>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60" s="54">
+        <v>57</v>
+      </c>
+      <c r="B60" s="55" t="s">
+        <v>203</v>
+      </c>
+      <c r="C60" s="55" t="s">
+        <v>119</v>
+      </c>
+      <c r="D60" s="56">
+        <v>7</v>
+      </c>
+      <c r="E60" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F60" s="68" t="s">
+        <v>79</v>
+      </c>
+      <c r="G60" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H60" s="39"/>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" s="54">
+        <v>58</v>
+      </c>
+      <c r="B61" s="55" t="s">
+        <v>204</v>
+      </c>
+      <c r="C61" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="D61" s="56">
+        <v>8</v>
+      </c>
+      <c r="E61" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F61" s="68" t="s">
+        <v>79</v>
+      </c>
+      <c r="G61" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H61" s="39"/>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62" s="54">
+        <v>59</v>
+      </c>
+      <c r="B62" s="55" t="s">
+        <v>205</v>
+      </c>
+      <c r="C62" s="55" t="s">
+        <v>150</v>
+      </c>
+      <c r="D62" s="56">
+        <v>10</v>
+      </c>
+      <c r="E62" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F62" s="68" t="s">
+        <v>79</v>
+      </c>
+      <c r="G62" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H62" s="39"/>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63" s="54">
+        <v>60</v>
+      </c>
+      <c r="B63" s="55" t="s">
+        <v>206</v>
+      </c>
+      <c r="C63" s="55" t="s">
+        <v>150</v>
+      </c>
+      <c r="D63" s="56">
+        <v>10</v>
+      </c>
+      <c r="E63" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F63" s="68" t="s">
+        <v>79</v>
+      </c>
+      <c r="G63" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H63" s="39"/>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64" s="54">
+        <v>61</v>
+      </c>
+      <c r="B64" s="55" t="s">
+        <v>207</v>
+      </c>
+      <c r="C64" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="D64" s="56">
+        <v>8</v>
+      </c>
+      <c r="E64" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F64" s="58" t="s">
+        <v>157</v>
+      </c>
+      <c r="G64" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H64" s="43"/>
+    </row>
+    <row r="65" spans="1:8" ht="69">
+      <c r="A65" s="59">
+        <v>62</v>
+      </c>
+      <c r="B65" s="60" t="s">
+        <v>27</v>
+      </c>
+      <c r="C65" s="71" t="s">
+        <v>41</v>
+      </c>
+      <c r="D65" s="61">
+        <v>3</v>
+      </c>
+      <c r="E65" s="62" t="s">
+        <v>114</v>
+      </c>
+      <c r="F65" s="63" t="s">
+        <v>208</v>
+      </c>
+      <c r="G65" s="40" t="s">
+        <v>209</v>
+      </c>
+      <c r="H65" s="39" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="55.2">
+      <c r="A66" s="54">
+        <v>63</v>
+      </c>
+      <c r="B66" s="55" t="s">
+        <v>211</v>
+      </c>
+      <c r="C66" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="D66" s="56">
+        <v>1</v>
+      </c>
+      <c r="E66" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F66" s="68" t="s">
+        <v>212</v>
+      </c>
+      <c r="G66" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H66" s="39"/>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="A67" s="54">
+        <v>64</v>
+      </c>
+      <c r="B67" s="55" t="s">
+        <v>213</v>
+      </c>
+      <c r="C67" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="D67" s="56">
+        <v>10</v>
+      </c>
+      <c r="E67" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F67" s="68" t="s">
+        <v>79</v>
+      </c>
+      <c r="G67" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H67" s="39"/>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="A68" s="54">
+        <v>65</v>
+      </c>
+      <c r="B68" s="55" t="s">
+        <v>214</v>
+      </c>
+      <c r="C68" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="D68" s="56">
+        <v>40</v>
+      </c>
+      <c r="E68" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F68" s="58" t="s">
+        <v>79</v>
+      </c>
+      <c r="G68" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H68" s="39"/>
+    </row>
+    <row r="69" spans="1:8" ht="41.4">
+      <c r="A69" s="54">
+        <v>66</v>
+      </c>
+      <c r="B69" s="55" t="s">
+        <v>215</v>
+      </c>
+      <c r="C69" s="69" t="s">
+        <v>41</v>
+      </c>
+      <c r="D69" s="72">
+        <v>1</v>
+      </c>
+      <c r="E69" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F69" s="68" t="s">
+        <v>216</v>
+      </c>
+      <c r="G69" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H69" s="44"/>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="A70" s="54">
+        <v>67</v>
+      </c>
+      <c r="B70" s="55" t="s">
+        <v>217</v>
+      </c>
+      <c r="C70" s="69" t="s">
+        <v>41</v>
+      </c>
+      <c r="D70" s="56">
+        <v>6</v>
+      </c>
+      <c r="E70" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F70" s="68" t="s">
+        <v>79</v>
+      </c>
+      <c r="G70" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="H70" s="45"/>
+    </row>
+    <row r="71" spans="1:8" ht="16.8" thickBot="1">
+      <c r="A71" s="54">
+        <v>68</v>
+      </c>
+      <c r="B71" s="55" t="s">
+        <v>218</v>
+      </c>
+      <c r="C71" s="55" t="s">
+        <v>150</v>
+      </c>
+      <c r="D71" s="56">
+        <v>10</v>
+      </c>
+      <c r="E71" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F71" s="73" t="s">
+        <v>79</v>
+      </c>
+      <c r="G71" s="46" t="s">
+        <v>112</v>
+      </c>
+      <c r="H71" s="45"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H26:H27"/>
+  </mergeCells>
+  <phoneticPr fontId="10" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A3" location="總表!A1" display="return" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B66300-3859-4B06-8E4B-B3D1526EF6DA}">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.2"/>
+  <cols>
+    <col min="1" max="1" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="78" t="s">
+        <v>219</v>
+      </c>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="77"/>
+    </row>
+    <row r="2" spans="1:8" ht="16.8" thickBot="1">
+      <c r="A2" s="78"/>
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="77"/>
+    </row>
+    <row r="3" spans="1:8" ht="27.6">
+      <c r="A3" s="82" t="s">
+        <v>220</v>
+      </c>
+      <c r="B3" s="82" t="s">
+        <v>221</v>
+      </c>
+      <c r="C3" s="82" t="s">
+        <v>222</v>
+      </c>
+      <c r="D3" s="82" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="82" t="s">
+        <v>223</v>
+      </c>
+      <c r="F3" s="81" t="s">
+        <v>107</v>
+      </c>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="83">
+        <v>1</v>
+      </c>
+      <c r="B4" s="83" t="s">
+        <v>224</v>
+      </c>
+      <c r="C4" s="83" t="s">
+        <v>225</v>
+      </c>
+      <c r="D4" s="83">
+        <v>12</v>
+      </c>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="83">
+        <v>2</v>
+      </c>
+      <c r="B5" s="83" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" s="83" t="s">
+        <v>225</v>
+      </c>
+      <c r="D5" s="83">
+        <v>12</v>
+      </c>
+      <c r="E5" s="83"/>
+      <c r="F5" s="83"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="75"/>
+    </row>
+    <row r="6" spans="1:8" ht="317.39999999999998">
+      <c r="A6" s="83">
+        <v>3</v>
+      </c>
+      <c r="B6" s="83" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="83" t="s">
+        <v>225</v>
+      </c>
+      <c r="D6" s="83">
+        <v>1</v>
+      </c>
+      <c r="E6" s="84"/>
+      <c r="F6" s="74" t="s">
+        <v>226</v>
+      </c>
+      <c r="G6" s="75"/>
+      <c r="H6" s="75"/>
+    </row>
+    <row r="7" spans="1:8" ht="27.6">
+      <c r="A7" s="83">
         <v>4</v>
       </c>
-      <c r="F2" s="31">
-        <v>0</v>
-      </c>
-      <c r="G2" s="31">
-        <v>4</v>
-      </c>
-      <c r="H2" s="32"/>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="31">
-        <v>2</v>
-      </c>
-      <c r="B3" s="31" t="s">
-        <v>89</v>
-      </c>
-      <c r="C3" s="31" t="s">
-        <v>90</v>
-      </c>
-      <c r="D3" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="E3" s="31">
-        <v>14</v>
-      </c>
-      <c r="F3" s="31">
-        <f>G2</f>
-        <v>4</v>
-      </c>
-      <c r="G3" s="31">
-        <f>F3+E3</f>
-        <v>18</v>
-      </c>
-      <c r="H3" s="32"/>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="31">
-        <v>3</v>
-      </c>
-      <c r="B4" s="31" t="s">
-        <v>92</v>
-      </c>
-      <c r="C4" s="31" t="s">
-        <v>93</v>
-      </c>
-      <c r="D4" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="E4" s="31">
-        <v>13</v>
-      </c>
-      <c r="F4" s="31">
-        <f t="shared" ref="F4:F11" si="0">G3</f>
-        <v>18</v>
-      </c>
-      <c r="G4" s="31">
-        <f t="shared" ref="G4:G11" si="1">F4+E4</f>
-        <v>31</v>
-      </c>
-      <c r="H4" s="32"/>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="31">
-        <v>4</v>
-      </c>
-      <c r="B5" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="C5" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="D5" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="E5" s="31">
+      <c r="B7" s="83" t="s">
+        <v>118</v>
+      </c>
+      <c r="C7" s="83" t="s">
+        <v>225</v>
+      </c>
+      <c r="D7" s="83">
         <v>7</v>
       </c>
-      <c r="F5" s="31">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="G5" s="31">
-        <f t="shared" si="1"/>
-        <v>38</v>
-      </c>
-      <c r="H5" s="32"/>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="31">
+      <c r="E7" s="83" t="s">
+        <v>227</v>
+      </c>
+      <c r="F7" s="85" t="s">
+        <v>228</v>
+      </c>
+      <c r="G7" s="75"/>
+      <c r="H7" s="75"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="83">
         <v>5</v>
       </c>
-      <c r="B6" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="C6" s="31" t="s">
-        <v>97</v>
-      </c>
-      <c r="D6" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="E6" s="30">
-        <v>59</v>
-      </c>
-      <c r="F6" s="31">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-      <c r="G6" s="31">
-        <f t="shared" si="1"/>
-        <v>97</v>
-      </c>
-      <c r="H6" s="32"/>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="31">
+      <c r="B8" s="83" t="s">
+        <v>127</v>
+      </c>
+      <c r="C8" s="83" t="s">
+        <v>225</v>
+      </c>
+      <c r="D8" s="83">
+        <v>15</v>
+      </c>
+      <c r="E8" s="83"/>
+      <c r="F8" s="85"/>
+      <c r="G8" s="75"/>
+      <c r="H8" s="75"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="83">
         <v>6</v>
       </c>
-      <c r="B7" s="31" t="s">
-        <v>98</v>
-      </c>
-      <c r="C7" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="D7" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="E7" s="31">
-        <v>35</v>
-      </c>
-      <c r="F7" s="31">
-        <f t="shared" si="0"/>
-        <v>97</v>
-      </c>
-      <c r="G7" s="31">
-        <f t="shared" si="1"/>
-        <v>132</v>
-      </c>
-      <c r="H7" s="32"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="31">
+      <c r="B9" s="83" t="s">
+        <v>130</v>
+      </c>
+      <c r="C9" s="83" t="s">
+        <v>225</v>
+      </c>
+      <c r="D9" s="83">
+        <v>40</v>
+      </c>
+      <c r="E9" s="83"/>
+      <c r="F9" s="85"/>
+      <c r="G9" s="75"/>
+      <c r="H9" s="75"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="83">
         <v>7</v>
       </c>
-      <c r="B8" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="C8" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="D8" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="E8" s="31">
-        <v>59</v>
-      </c>
-      <c r="F8" s="31">
-        <f t="shared" si="0"/>
-        <v>132</v>
-      </c>
-      <c r="G8" s="31">
-        <f t="shared" si="1"/>
-        <v>191</v>
-      </c>
-      <c r="H8" s="32"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="31">
+      <c r="B10" s="83" t="s">
+        <v>137</v>
+      </c>
+      <c r="C10" s="83" t="s">
+        <v>225</v>
+      </c>
+      <c r="D10" s="83">
+        <v>9</v>
+      </c>
+      <c r="E10" s="83"/>
+      <c r="F10" s="85"/>
+      <c r="G10" s="75"/>
+      <c r="H10" s="75"/>
+    </row>
+    <row r="11" spans="1:8" ht="27.6">
+      <c r="A11" s="83">
         <v>8</v>
       </c>
-      <c r="B9" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="C9" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="D9" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="E9" s="31">
-        <v>5</v>
-      </c>
-      <c r="F9" s="31">
-        <f t="shared" si="0"/>
-        <v>191</v>
-      </c>
-      <c r="G9" s="31">
-        <f t="shared" si="1"/>
-        <v>196</v>
-      </c>
-      <c r="H9" s="32"/>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="31">
+      <c r="B11" s="83" t="s">
+        <v>140</v>
+      </c>
+      <c r="C11" s="83" t="s">
+        <v>225</v>
+      </c>
+      <c r="D11" s="83">
+        <v>7</v>
+      </c>
+      <c r="E11" s="83" t="s">
+        <v>227</v>
+      </c>
+      <c r="F11" s="85" t="s">
+        <v>228</v>
+      </c>
+      <c r="G11" s="75"/>
+      <c r="H11" s="75"/>
+    </row>
+    <row r="12" spans="1:8" ht="41.4">
+      <c r="A12" s="83">
         <v>9</v>
       </c>
-      <c r="B10" s="31" t="s">
-        <v>104</v>
-      </c>
-      <c r="C10" s="31" t="s">
-        <v>105</v>
-      </c>
-      <c r="D10" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="E10" s="31">
-        <v>8</v>
-      </c>
-      <c r="F10" s="31">
-        <f t="shared" si="0"/>
-        <v>196</v>
-      </c>
-      <c r="G10" s="31">
-        <f t="shared" si="1"/>
-        <v>204</v>
-      </c>
-      <c r="H10" s="32"/>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="31">
-        <v>10</v>
-      </c>
-      <c r="B11" s="31" t="s">
-        <v>106</v>
-      </c>
-      <c r="C11" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="D11" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="E11" s="31">
-        <v>2</v>
-      </c>
-      <c r="F11" s="31">
-        <f t="shared" si="0"/>
-        <v>204</v>
-      </c>
-      <c r="G11" s="31">
-        <f t="shared" si="1"/>
-        <v>206</v>
-      </c>
-      <c r="H11" s="32"/>
+      <c r="B12" s="83" t="s">
+        <v>141</v>
+      </c>
+      <c r="C12" s="83" t="s">
+        <v>225</v>
+      </c>
+      <c r="D12" s="83">
+        <v>7</v>
+      </c>
+      <c r="E12" s="83" t="s">
+        <v>227</v>
+      </c>
+      <c r="F12" s="85" t="s">
+        <v>228</v>
+      </c>
+      <c r="G12" s="75"/>
+      <c r="H12" s="75"/>
     </row>
   </sheetData>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Auto-committed on 2021/12/28 週二
Former-commit-id: a88688ed944765797673b21a468f0aa9f1ec8b15
</commit_message>
<xml_diff>
--- a/Program/Other/URS會議審查紀錄/DbLayouts/L4-批次作業/BankRemit.xlsx
+++ b/Program/Other/URS會議審查紀錄/DbLayouts/L4-批次作業/BankRemit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\SKL\DB\GenTables\L4-批次作業\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5655F6-2551-4EDC-989C-66114C1289AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C627FB94-BA4E-4276-B544-E13687E0F89A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DBD" sheetId="1" r:id="rId1"/>
@@ -415,30 +415,6 @@
   </si>
   <si>
     <t>PayCode</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>I:建檔
-O:確認
-C:建檔取消
-A:已開票
-D:支票到期
-B:退件
-S:請款單位擋匯
-T:網銀擋匯
-W:匯款途中
-F:匯款失敗
-H:支票兌領/匯款成功
-R:退匯/退回情況改變成作廢
-L:支票掛失
-V:支票作廢
-J:空白票遺失
-Z:逾一年未兌領
-Y:逾二年未兌領
-P:繳款成功
-X:付款沖回
-Q:AML相似名單確認中
-U:禁止交易(AML)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -1018,6 +994,31 @@
   <si>
     <t>CustNo = ,AND FacmNo = ,AND BormNo = ,AND DrawdownCode =</t>
     <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>CdCode:PayCode
+I:建檔
+O:確認
+C:建檔取消
+A:已開票
+D:支票到期
+B:退件
+S:請款單位擋匯
+T:網銀擋匯
+W:匯款途中
+F:匯款失敗
+H:支票兌領/匯款成功
+R:退匯/退回情況改變成作廢
+L:支票掛失
+V:支票作廢
+J:空白票遺失
+Z:逾一年未兌領
+Y:逾二年未兌領
+P:繳款成功
+X:付款沖回
+Q:AML相似名單確認中
+U:禁止交易(AML)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2021,8 +2022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.44140625" defaultRowHeight="16.2"/>
@@ -2512,7 +2513,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="340.2">
+    <row r="28" spans="1:8" ht="356.4">
       <c r="A28" s="18">
         <v>20</v>
       </c>
@@ -2530,7 +2531,7 @@
       </c>
       <c r="F28" s="18"/>
       <c r="G28" s="23" t="s">
-        <v>99</v>
+        <v>233</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -2626,7 +2627,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
@@ -2690,21 +2691,21 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>231</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>232</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -2736,7 +2737,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="48" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
@@ -2748,7 +2749,7 @@
     </row>
     <row r="2" spans="1:8" ht="16.8" thickBot="1">
       <c r="A2" s="48" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B2" s="30"/>
       <c r="C2" s="30"/>
@@ -2760,25 +2761,25 @@
     </row>
     <row r="3" spans="1:8" ht="41.4">
       <c r="A3" s="42" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="43" t="s">
+      <c r="C3" s="43" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="43" t="s">
+      <c r="D3" s="44" t="s">
         <v>104</v>
       </c>
-      <c r="D3" s="44" t="s">
+      <c r="E3" s="45" t="s">
         <v>105</v>
       </c>
-      <c r="E3" s="45" t="s">
+      <c r="F3" s="46" t="s">
         <v>106</v>
       </c>
-      <c r="F3" s="46" t="s">
+      <c r="G3" s="31" t="s">
         <v>107</v>
-      </c>
-      <c r="G3" s="31" t="s">
-        <v>108</v>
       </c>
       <c r="H3" s="47"/>
     </row>
@@ -2787,7 +2788,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C4" s="50" t="s">
         <v>41</v>
@@ -2796,13 +2797,13 @@
         <v>12</v>
       </c>
       <c r="E4" s="52" t="s">
+        <v>109</v>
+      </c>
+      <c r="F4" s="53" t="s">
         <v>110</v>
       </c>
-      <c r="F4" s="53" t="s">
-        <v>111</v>
-      </c>
       <c r="G4" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H4" s="33"/>
     </row>
@@ -2811,7 +2812,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C5" s="50" t="s">
         <v>41</v>
@@ -2820,13 +2821,13 @@
         <v>12</v>
       </c>
       <c r="E5" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F5" s="53" t="s">
         <v>79</v>
       </c>
       <c r="G5" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H5" s="34"/>
     </row>
@@ -2835,7 +2836,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C6" s="50" t="s">
         <v>41</v>
@@ -2844,13 +2845,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F6" s="53" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G6" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H6" s="34"/>
     </row>
@@ -2868,13 +2869,13 @@
         <v>1</v>
       </c>
       <c r="E7" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F7" s="53" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G7" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H7" s="34"/>
     </row>
@@ -2883,22 +2884,22 @@
         <v>5</v>
       </c>
       <c r="B8" s="50" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" s="50" t="s">
         <v>118</v>
-      </c>
-      <c r="C8" s="50" t="s">
-        <v>119</v>
       </c>
       <c r="D8" s="51">
         <v>7</v>
       </c>
       <c r="E8" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F8" s="53" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G8" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H8" s="34"/>
     </row>
@@ -2907,7 +2908,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="55" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C9" s="55" t="s">
         <v>41</v>
@@ -2916,13 +2917,13 @@
         <v>1</v>
       </c>
       <c r="E9" s="57" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F9" s="58" t="s">
+        <v>121</v>
+      </c>
+      <c r="G9" s="35" t="s">
         <v>122</v>
-      </c>
-      <c r="G9" s="35" t="s">
-        <v>123</v>
       </c>
       <c r="H9" s="34"/>
     </row>
@@ -2931,7 +2932,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="55" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C10" s="55" t="s">
         <v>41</v>
@@ -2940,13 +2941,13 @@
         <v>1</v>
       </c>
       <c r="E10" s="57" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F10" s="58" t="s">
+        <v>124</v>
+      </c>
+      <c r="G10" s="35" t="s">
         <v>125</v>
-      </c>
-      <c r="G10" s="35" t="s">
-        <v>126</v>
       </c>
       <c r="H10" s="34"/>
     </row>
@@ -2955,7 +2956,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="55" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C11" s="55" t="s">
         <v>41</v>
@@ -2964,16 +2965,16 @@
         <v>15</v>
       </c>
       <c r="E11" s="57" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F11" s="59" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G11" s="35" t="s">
+        <v>127</v>
+      </c>
+      <c r="H11" s="36" t="s">
         <v>128</v>
-      </c>
-      <c r="H11" s="36" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -2981,7 +2982,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="55" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C12" s="55" t="s">
         <v>41</v>
@@ -2990,13 +2991,13 @@
         <v>40</v>
       </c>
       <c r="E12" s="57" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F12" s="59" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G12" s="35" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H12" s="34"/>
     </row>
@@ -3005,7 +3006,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="55" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C13" s="55" t="s">
         <v>41</v>
@@ -3014,16 +3015,16 @@
         <v>45</v>
       </c>
       <c r="E13" s="57" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F13" s="59" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G13" s="37" t="s">
+        <v>132</v>
+      </c>
+      <c r="H13" s="34" t="s">
         <v>133</v>
-      </c>
-      <c r="H13" s="34" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="69">
@@ -3031,7 +3032,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="55" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C14" s="55" t="s">
         <v>41</v>
@@ -3040,13 +3041,13 @@
         <v>1</v>
       </c>
       <c r="E14" s="60" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F14" s="58" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G14" s="35" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H14" s="36"/>
     </row>
@@ -3055,7 +3056,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="50" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C15" s="50" t="s">
         <v>41</v>
@@ -3064,13 +3065,13 @@
         <v>9</v>
       </c>
       <c r="E15" s="61" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F15" s="53" t="s">
         <v>79</v>
       </c>
       <c r="G15" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H15" s="34"/>
     </row>
@@ -3079,25 +3080,25 @@
         <v>13</v>
       </c>
       <c r="B16" s="55" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C16" s="55" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D16" s="56">
         <v>7</v>
       </c>
       <c r="E16" s="60" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F16" s="59" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G16" s="35" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H16" s="34" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -3105,22 +3106,22 @@
         <v>14</v>
       </c>
       <c r="B17" s="50" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C17" s="50" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D17" s="51">
         <v>7</v>
       </c>
       <c r="E17" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F17" s="53" t="s">
         <v>79</v>
       </c>
       <c r="G17" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H17" s="34"/>
     </row>
@@ -3129,22 +3130,22 @@
         <v>15</v>
       </c>
       <c r="B18" s="50" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C18" s="50" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D18" s="51">
         <v>7</v>
       </c>
       <c r="E18" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F18" s="53" t="s">
         <v>79</v>
       </c>
       <c r="G18" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H18" s="34"/>
     </row>
@@ -3153,7 +3154,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="55" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C19" s="55" t="s">
         <v>41</v>
@@ -3162,13 +3163,13 @@
         <v>3</v>
       </c>
       <c r="E19" s="57" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F19" s="59" t="s">
+        <v>142</v>
+      </c>
+      <c r="G19" s="35" t="s">
         <v>143</v>
-      </c>
-      <c r="G19" s="35" t="s">
-        <v>144</v>
       </c>
       <c r="H19" s="34"/>
     </row>
@@ -3177,7 +3178,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="55" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C20" s="55" t="s">
         <v>41</v>
@@ -3186,13 +3187,13 @@
         <v>4</v>
       </c>
       <c r="E20" s="57" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F20" s="59" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G20" s="35" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H20" s="34"/>
     </row>
@@ -3201,7 +3202,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="55" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C21" s="55" t="s">
         <v>41</v>
@@ -3210,13 +3211,13 @@
         <v>16</v>
       </c>
       <c r="E21" s="57" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F21" s="59" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G21" s="35" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H21" s="34"/>
     </row>
@@ -3225,22 +3226,22 @@
         <v>19</v>
       </c>
       <c r="B22" s="55" t="s">
+        <v>148</v>
+      </c>
+      <c r="C22" s="55" t="s">
         <v>149</v>
       </c>
-      <c r="C22" s="55" t="s">
+      <c r="D22" s="62" t="s">
         <v>150</v>
       </c>
-      <c r="D22" s="62" t="s">
+      <c r="E22" s="57" t="s">
+        <v>113</v>
+      </c>
+      <c r="F22" s="59" t="s">
+        <v>107</v>
+      </c>
+      <c r="G22" s="35" t="s">
         <v>151</v>
-      </c>
-      <c r="E22" s="57" t="s">
-        <v>114</v>
-      </c>
-      <c r="F22" s="59" t="s">
-        <v>108</v>
-      </c>
-      <c r="G22" s="35" t="s">
-        <v>152</v>
       </c>
       <c r="H22" s="34"/>
     </row>
@@ -3249,7 +3250,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="50" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C23" s="50" t="s">
         <v>41</v>
@@ -3258,13 +3259,13 @@
         <v>8</v>
       </c>
       <c r="E23" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F23" s="63" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G23" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H23" s="34"/>
     </row>
@@ -3273,7 +3274,7 @@
         <v>21</v>
       </c>
       <c r="B24" s="50" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C24" s="50" t="s">
         <v>41</v>
@@ -3282,13 +3283,13 @@
         <v>2</v>
       </c>
       <c r="E24" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F24" s="63" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G24" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H24" s="34"/>
     </row>
@@ -3297,7 +3298,7 @@
         <v>22</v>
       </c>
       <c r="B25" s="50" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C25" s="50" t="s">
         <v>41</v>
@@ -3306,13 +3307,13 @@
         <v>8</v>
       </c>
       <c r="E25" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F25" s="63" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G25" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H25" s="34"/>
     </row>
@@ -3321,22 +3322,22 @@
         <v>23</v>
       </c>
       <c r="B26" s="50" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C26" s="50" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D26" s="51">
         <v>7</v>
       </c>
       <c r="E26" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F26" s="63" t="s">
         <v>79</v>
       </c>
       <c r="G26" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H26" s="85"/>
     </row>
@@ -3345,22 +3346,22 @@
         <v>24</v>
       </c>
       <c r="B27" s="50" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C27" s="50" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D27" s="51">
         <v>7</v>
       </c>
       <c r="E27" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F27" s="63" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G27" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H27" s="85"/>
     </row>
@@ -3369,7 +3370,7 @@
         <v>25</v>
       </c>
       <c r="B28" s="50" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C28" s="50" t="s">
         <v>41</v>
@@ -3378,13 +3379,13 @@
         <v>8</v>
       </c>
       <c r="E28" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F28" s="63" t="s">
         <v>79</v>
       </c>
       <c r="G28" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H28" s="34"/>
     </row>
@@ -3393,22 +3394,22 @@
         <v>26</v>
       </c>
       <c r="B29" s="50" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C29" s="50" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D29" s="51">
         <v>10</v>
       </c>
       <c r="E29" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F29" s="63" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G29" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H29" s="34"/>
     </row>
@@ -3417,22 +3418,22 @@
         <v>27</v>
       </c>
       <c r="B30" s="50" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C30" s="50" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D30" s="51">
         <v>7</v>
       </c>
       <c r="E30" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F30" s="63" t="s">
         <v>79</v>
       </c>
       <c r="G30" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H30" s="34"/>
     </row>
@@ -3441,7 +3442,7 @@
         <v>28</v>
       </c>
       <c r="B31" s="50" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C31" s="50" t="s">
         <v>41</v>
@@ -3450,13 +3451,13 @@
         <v>1</v>
       </c>
       <c r="E31" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F31" s="63" t="s">
         <v>79</v>
       </c>
       <c r="G31" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H31" s="34"/>
     </row>
@@ -3465,7 +3466,7 @@
         <v>29</v>
       </c>
       <c r="B32" s="50" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C32" s="50" t="s">
         <v>41</v>
@@ -3474,13 +3475,13 @@
         <v>1</v>
       </c>
       <c r="E32" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F32" s="63" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G32" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H32" s="34"/>
     </row>
@@ -3489,7 +3490,7 @@
         <v>30</v>
       </c>
       <c r="B33" s="50" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C33" s="50" t="s">
         <v>41</v>
@@ -3498,13 +3499,13 @@
         <v>1</v>
       </c>
       <c r="E33" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F33" s="63" t="s">
         <v>79</v>
       </c>
       <c r="G33" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H33" s="34"/>
     </row>
@@ -3513,7 +3514,7 @@
         <v>31</v>
       </c>
       <c r="B34" s="55" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C34" s="55" t="s">
         <v>41</v>
@@ -3522,13 +3523,13 @@
         <v>12</v>
       </c>
       <c r="E34" s="57" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F34" s="58" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G34" s="35" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H34" s="34"/>
     </row>
@@ -3537,7 +3538,7 @@
         <v>32</v>
       </c>
       <c r="B35" s="50" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C35" s="50" t="s">
         <v>41</v>
@@ -3546,13 +3547,13 @@
         <v>6</v>
       </c>
       <c r="E35" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F35" s="53" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G35" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H35" s="34"/>
     </row>
@@ -3561,7 +3562,7 @@
         <v>33</v>
       </c>
       <c r="B36" s="50" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C36" s="50" t="s">
         <v>41</v>
@@ -3570,13 +3571,13 @@
         <v>1</v>
       </c>
       <c r="E36" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F36" s="53" t="s">
         <v>79</v>
       </c>
       <c r="G36" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H36" s="34"/>
     </row>
@@ -3585,7 +3586,7 @@
         <v>34</v>
       </c>
       <c r="B37" s="50" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C37" s="50" t="s">
         <v>41</v>
@@ -3594,13 +3595,13 @@
         <v>1</v>
       </c>
       <c r="E37" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F37" s="63" t="s">
         <v>79</v>
       </c>
       <c r="G37" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H37" s="34"/>
     </row>
@@ -3609,7 +3610,7 @@
         <v>35</v>
       </c>
       <c r="B38" s="50" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C38" s="50" t="s">
         <v>41</v>
@@ -3618,13 +3619,13 @@
         <v>1</v>
       </c>
       <c r="E38" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F38" s="63" t="s">
         <v>79</v>
       </c>
       <c r="G38" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H38" s="34"/>
     </row>
@@ -3633,7 +3634,7 @@
         <v>36</v>
       </c>
       <c r="B39" s="50" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C39" s="50" t="s">
         <v>41</v>
@@ -3642,13 +3643,13 @@
         <v>12</v>
       </c>
       <c r="E39" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F39" s="53" t="s">
         <v>79</v>
       </c>
       <c r="G39" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H39" s="34"/>
     </row>
@@ -3657,7 +3658,7 @@
         <v>37</v>
       </c>
       <c r="B40" s="55" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C40" s="55" t="s">
         <v>41</v>
@@ -3666,16 +3667,16 @@
         <v>1</v>
       </c>
       <c r="E40" s="57" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F40" s="58" t="s">
+        <v>176</v>
+      </c>
+      <c r="G40" s="35" t="s">
         <v>177</v>
       </c>
-      <c r="G40" s="35" t="s">
+      <c r="H40" s="33" t="s">
         <v>178</v>
-      </c>
-      <c r="H40" s="33" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -3683,7 +3684,7 @@
         <v>38</v>
       </c>
       <c r="B41" s="50" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C41" s="50" t="s">
         <v>41</v>
@@ -3692,13 +3693,13 @@
         <v>1</v>
       </c>
       <c r="E41" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F41" s="63" t="s">
         <v>79</v>
       </c>
       <c r="G41" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H41" s="34"/>
     </row>
@@ -3707,7 +3708,7 @@
         <v>39</v>
       </c>
       <c r="B42" s="50" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C42" s="50" t="s">
         <v>41</v>
@@ -3716,13 +3717,13 @@
         <v>6</v>
       </c>
       <c r="E42" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F42" s="63" t="s">
         <v>79</v>
       </c>
       <c r="G42" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H42" s="34"/>
     </row>
@@ -3731,22 +3732,22 @@
         <v>40</v>
       </c>
       <c r="B43" s="50" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C43" s="50" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D43" s="51">
         <v>10</v>
       </c>
       <c r="E43" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F43" s="53" t="s">
         <v>79</v>
       </c>
       <c r="G43" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H43" s="34"/>
     </row>
@@ -3755,7 +3756,7 @@
         <v>41</v>
       </c>
       <c r="B44" s="50" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C44" s="50" t="s">
         <v>41</v>
@@ -3764,13 +3765,13 @@
         <v>7</v>
       </c>
       <c r="E44" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F44" s="53" t="s">
         <v>79</v>
       </c>
       <c r="G44" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H44" s="34"/>
     </row>
@@ -3779,7 +3780,7 @@
         <v>42</v>
       </c>
       <c r="B45" s="50" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C45" s="50" t="s">
         <v>41</v>
@@ -3788,13 +3789,13 @@
         <v>10</v>
       </c>
       <c r="E45" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F45" s="53" t="s">
         <v>79</v>
       </c>
       <c r="G45" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H45" s="34"/>
     </row>
@@ -3803,22 +3804,22 @@
         <v>43</v>
       </c>
       <c r="B46" s="50" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C46" s="50" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D46" s="51">
         <v>7</v>
       </c>
       <c r="E46" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F46" s="53" t="s">
         <v>79</v>
       </c>
       <c r="G46" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H46" s="34"/>
     </row>
@@ -3827,7 +3828,7 @@
         <v>44</v>
       </c>
       <c r="B47" s="50" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C47" s="50" t="s">
         <v>41</v>
@@ -3836,13 +3837,13 @@
         <v>12</v>
       </c>
       <c r="E47" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F47" s="53" t="s">
         <v>79</v>
       </c>
       <c r="G47" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H47" s="34"/>
     </row>
@@ -3851,7 +3852,7 @@
         <v>45</v>
       </c>
       <c r="B48" s="50" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C48" s="50" t="s">
         <v>41</v>
@@ -3860,13 +3861,13 @@
         <v>1</v>
       </c>
       <c r="E48" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F48" s="63" t="s">
         <v>79</v>
       </c>
       <c r="G48" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H48" s="34"/>
     </row>
@@ -3875,7 +3876,7 @@
         <v>46</v>
       </c>
       <c r="B49" s="50" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C49" s="50" t="s">
         <v>41</v>
@@ -3884,13 +3885,13 @@
         <v>5</v>
       </c>
       <c r="E49" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F49" s="53" t="s">
         <v>79</v>
       </c>
       <c r="G49" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H49" s="34"/>
     </row>
@@ -3899,7 +3900,7 @@
         <v>47</v>
       </c>
       <c r="B50" s="50" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C50" s="50" t="s">
         <v>41</v>
@@ -3908,13 +3909,13 @@
         <v>80</v>
       </c>
       <c r="E50" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F50" s="53" t="s">
         <v>79</v>
       </c>
       <c r="G50" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H50" s="34"/>
     </row>
@@ -3923,7 +3924,7 @@
         <v>48</v>
       </c>
       <c r="B51" s="50" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C51" s="50" t="s">
         <v>41</v>
@@ -3932,13 +3933,13 @@
         <v>1</v>
       </c>
       <c r="E51" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F51" s="63" t="s">
         <v>79</v>
       </c>
       <c r="G51" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H51" s="34"/>
     </row>
@@ -3947,7 +3948,7 @@
         <v>49</v>
       </c>
       <c r="B52" s="55" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C52" s="55" t="s">
         <v>41</v>
@@ -3956,13 +3957,13 @@
         <v>10</v>
       </c>
       <c r="E52" s="57" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F52" s="59" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G52" s="35" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H52" s="34"/>
     </row>
@@ -3971,7 +3972,7 @@
         <v>50</v>
       </c>
       <c r="B53" s="50" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C53" s="64" t="s">
         <v>41</v>
@@ -3980,13 +3981,13 @@
         <v>12</v>
       </c>
       <c r="E53" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F53" s="53" t="s">
         <v>79</v>
       </c>
       <c r="G53" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H53" s="34"/>
     </row>
@@ -3995,7 +3996,7 @@
         <v>51</v>
       </c>
       <c r="B54" s="50" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C54" s="64" t="s">
         <v>41</v>
@@ -4004,13 +4005,13 @@
         <v>1</v>
       </c>
       <c r="E54" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F54" s="63" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G54" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H54" s="34"/>
     </row>
@@ -4019,7 +4020,7 @@
         <v>52</v>
       </c>
       <c r="B55" s="50" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C55" s="50" t="s">
         <v>41</v>
@@ -4028,13 +4029,13 @@
         <v>2</v>
       </c>
       <c r="E55" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F55" s="63" t="s">
         <v>79</v>
       </c>
       <c r="G55" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H55" s="34"/>
     </row>
@@ -4043,7 +4044,7 @@
         <v>53</v>
       </c>
       <c r="B56" s="49" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C56" s="49" t="s">
         <v>41</v>
@@ -4052,13 +4053,13 @@
         <v>12</v>
       </c>
       <c r="E56" s="52" t="s">
+        <v>109</v>
+      </c>
+      <c r="F56" s="63" t="s">
         <v>110</v>
       </c>
-      <c r="F56" s="63" t="s">
-        <v>111</v>
-      </c>
       <c r="G56" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H56" s="34"/>
     </row>
@@ -4067,7 +4068,7 @@
         <v>54</v>
       </c>
       <c r="B57" s="55" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C57" s="55" t="s">
         <v>41</v>
@@ -4076,16 +4077,16 @@
         <v>12</v>
       </c>
       <c r="E57" s="57" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F57" s="59" t="s">
+        <v>198</v>
+      </c>
+      <c r="G57" s="35" t="s">
         <v>199</v>
       </c>
-      <c r="G57" s="35" t="s">
-        <v>200</v>
-      </c>
       <c r="H57" s="34" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -4093,22 +4094,22 @@
         <v>55</v>
       </c>
       <c r="B58" s="50" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C58" s="50" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D58" s="51">
         <v>7</v>
       </c>
       <c r="E58" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F58" s="63" t="s">
         <v>79</v>
       </c>
       <c r="G58" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H58" s="34"/>
     </row>
@@ -4117,7 +4118,7 @@
         <v>56</v>
       </c>
       <c r="B59" s="50" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C59" s="50" t="s">
         <v>41</v>
@@ -4126,13 +4127,13 @@
         <v>8</v>
       </c>
       <c r="E59" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F59" s="63" t="s">
         <v>79</v>
       </c>
       <c r="G59" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H59" s="34"/>
     </row>
@@ -4141,22 +4142,22 @@
         <v>57</v>
       </c>
       <c r="B60" s="50" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C60" s="50" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D60" s="51">
         <v>7</v>
       </c>
       <c r="E60" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F60" s="63" t="s">
         <v>79</v>
       </c>
       <c r="G60" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H60" s="34"/>
     </row>
@@ -4165,7 +4166,7 @@
         <v>58</v>
       </c>
       <c r="B61" s="50" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C61" s="50" t="s">
         <v>41</v>
@@ -4174,13 +4175,13 @@
         <v>8</v>
       </c>
       <c r="E61" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F61" s="63" t="s">
         <v>79</v>
       </c>
       <c r="G61" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H61" s="34"/>
     </row>
@@ -4189,22 +4190,22 @@
         <v>59</v>
       </c>
       <c r="B62" s="50" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C62" s="50" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D62" s="51">
         <v>10</v>
       </c>
       <c r="E62" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F62" s="63" t="s">
         <v>79</v>
       </c>
       <c r="G62" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H62" s="34"/>
     </row>
@@ -4213,22 +4214,22 @@
         <v>60</v>
       </c>
       <c r="B63" s="50" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C63" s="50" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D63" s="51">
         <v>10</v>
       </c>
       <c r="E63" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F63" s="63" t="s">
         <v>79</v>
       </c>
       <c r="G63" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H63" s="34"/>
     </row>
@@ -4237,7 +4238,7 @@
         <v>61</v>
       </c>
       <c r="B64" s="50" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C64" s="50" t="s">
         <v>41</v>
@@ -4246,13 +4247,13 @@
         <v>8</v>
       </c>
       <c r="E64" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F64" s="53" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G64" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H64" s="38"/>
     </row>
@@ -4270,16 +4271,16 @@
         <v>3</v>
       </c>
       <c r="E65" s="57" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F65" s="58" t="s">
+        <v>207</v>
+      </c>
+      <c r="G65" s="35" t="s">
         <v>208</v>
       </c>
-      <c r="G65" s="35" t="s">
+      <c r="H65" s="34" t="s">
         <v>209</v>
-      </c>
-      <c r="H65" s="34" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -4287,7 +4288,7 @@
         <v>63</v>
       </c>
       <c r="B66" s="50" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C66" s="50" t="s">
         <v>41</v>
@@ -4296,13 +4297,13 @@
         <v>1</v>
       </c>
       <c r="E66" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F66" s="63" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G66" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H66" s="34"/>
     </row>
@@ -4311,7 +4312,7 @@
         <v>64</v>
       </c>
       <c r="B67" s="50" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C67" s="50" t="s">
         <v>41</v>
@@ -4320,13 +4321,13 @@
         <v>10</v>
       </c>
       <c r="E67" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F67" s="63" t="s">
         <v>79</v>
       </c>
       <c r="G67" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H67" s="34"/>
     </row>
@@ -4335,7 +4336,7 @@
         <v>65</v>
       </c>
       <c r="B68" s="50" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C68" s="50" t="s">
         <v>41</v>
@@ -4344,13 +4345,13 @@
         <v>40</v>
       </c>
       <c r="E68" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F68" s="53" t="s">
         <v>79</v>
       </c>
       <c r="G68" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H68" s="34"/>
     </row>
@@ -4359,7 +4360,7 @@
         <v>66</v>
       </c>
       <c r="B69" s="50" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C69" s="64" t="s">
         <v>41</v>
@@ -4368,13 +4369,13 @@
         <v>1</v>
       </c>
       <c r="E69" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F69" s="63" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G69" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H69" s="39"/>
     </row>
@@ -4383,7 +4384,7 @@
         <v>67</v>
       </c>
       <c r="B70" s="50" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C70" s="64" t="s">
         <v>41</v>
@@ -4392,13 +4393,13 @@
         <v>6</v>
       </c>
       <c r="E70" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F70" s="63" t="s">
         <v>79</v>
       </c>
       <c r="G70" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H70" s="40"/>
     </row>
@@ -4407,22 +4408,22 @@
         <v>68</v>
       </c>
       <c r="B71" s="50" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C71" s="50" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D71" s="51">
         <v>10</v>
       </c>
       <c r="E71" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F71" s="68" t="s">
         <v>79</v>
       </c>
       <c r="G71" s="41" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H71" s="40"/>
     </row>
@@ -4459,7 +4460,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="73" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B1" s="74"/>
       <c r="C1" s="74"/>
@@ -4481,22 +4482,22 @@
     </row>
     <row r="3" spans="1:8" ht="27.6">
       <c r="A3" s="77" t="s">
+        <v>219</v>
+      </c>
+      <c r="B3" s="77" t="s">
         <v>220</v>
       </c>
-      <c r="B3" s="77" t="s">
+      <c r="C3" s="77" t="s">
         <v>221</v>
-      </c>
-      <c r="C3" s="77" t="s">
-        <v>222</v>
       </c>
       <c r="D3" s="77" t="s">
         <v>14</v>
       </c>
       <c r="E3" s="77" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F3" s="76" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G3" s="70"/>
       <c r="H3" s="70"/>
@@ -4506,10 +4507,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="78" t="s">
+        <v>223</v>
+      </c>
+      <c r="C4" s="78" t="s">
         <v>224</v>
-      </c>
-      <c r="C4" s="78" t="s">
-        <v>225</v>
       </c>
       <c r="D4" s="78">
         <v>12</v>
@@ -4524,10 +4525,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="78" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C5" s="78" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D5" s="78">
         <v>12</v>
@@ -4545,14 +4546,14 @@
         <v>96</v>
       </c>
       <c r="C6" s="78" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D6" s="78">
         <v>1</v>
       </c>
       <c r="E6" s="79"/>
       <c r="F6" s="69" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G6" s="70"/>
       <c r="H6" s="70"/>
@@ -4562,19 +4563,19 @@
         <v>4</v>
       </c>
       <c r="B7" s="78" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C7" s="78" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D7" s="78">
         <v>7</v>
       </c>
       <c r="E7" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="F7" s="80" t="s">
         <v>227</v>
-      </c>
-      <c r="F7" s="80" t="s">
-        <v>228</v>
       </c>
       <c r="G7" s="70"/>
       <c r="H7" s="70"/>
@@ -4584,10 +4585,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="78" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C8" s="78" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D8" s="78">
         <v>15</v>
@@ -4602,10 +4603,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="78" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C9" s="78" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D9" s="78">
         <v>40</v>
@@ -4620,10 +4621,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="78" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C10" s="78" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D10" s="78">
         <v>9</v>
@@ -4638,19 +4639,19 @@
         <v>8</v>
       </c>
       <c r="B11" s="78" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C11" s="78" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D11" s="78">
         <v>7</v>
       </c>
       <c r="E11" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="F11" s="80" t="s">
         <v>227</v>
-      </c>
-      <c r="F11" s="80" t="s">
-        <v>228</v>
       </c>
       <c r="G11" s="70"/>
       <c r="H11" s="70"/>
@@ -4660,19 +4661,19 @@
         <v>9</v>
       </c>
       <c r="B12" s="78" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C12" s="78" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D12" s="78">
         <v>7</v>
       </c>
       <c r="E12" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="F12" s="80" t="s">
         <v>227</v>
-      </c>
-      <c r="F12" s="80" t="s">
-        <v>228</v>
       </c>
       <c r="G12" s="70"/>
       <c r="H12" s="70"/>

</xml_diff>